<commit_message>
Update list with companies coming in September
</commit_message>
<xml_diff>
--- a/Thapar BE_B Tech 2025 Placement Data.xlsx
+++ b/Thapar BE_B Tech 2025 Placement Data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="118">
   <si>
     <t>S No.</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Location</t>
   </si>
   <si>
+    <t>CG Cut</t>
+  </si>
+  <si>
     <t>JP Morgan</t>
   </si>
   <si>
@@ -70,15 +73,15 @@
     <t>Specialist Programmer</t>
   </si>
   <si>
+    <t>July</t>
+  </si>
+  <si>
     <t>Google</t>
   </si>
   <si>
     <t>SDE</t>
   </si>
   <si>
-    <t>July</t>
-  </si>
-  <si>
     <t>Bain</t>
   </si>
   <si>
@@ -127,6 +130,12 @@
     <t>Misc</t>
   </si>
   <si>
+    <t>Arista(Through ACE Certification Program)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>Cloudera</t>
   </si>
   <si>
@@ -154,6 +163,12 @@
     <t>AI Product Analyst</t>
   </si>
   <si>
+    <t>IBM</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
     <t>Playsimple</t>
   </si>
   <si>
@@ -286,6 +301,9 @@
     <t>ARM</t>
   </si>
   <si>
+    <t>Hardware</t>
+  </si>
+  <si>
     <t>Meesho</t>
   </si>
   <si>
@@ -305,6 +323,54 @@
   </si>
   <si>
     <t>Deloitte</t>
+  </si>
+  <si>
+    <t>Axtria</t>
+  </si>
+  <si>
+    <t>Verizon</t>
+  </si>
+  <si>
+    <t>Amadeus Labs</t>
+  </si>
+  <si>
+    <t>Honda</t>
+  </si>
+  <si>
+    <t>Signify</t>
+  </si>
+  <si>
+    <t>Assistant Dev Engineer</t>
+  </si>
+  <si>
+    <t>IDFC Bank</t>
+  </si>
+  <si>
+    <t>Associate Data Engineer</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t>September</t>
+    </r>
+  </si>
+  <si>
+    <t>GEP Worldwide</t>
+  </si>
+  <si>
+    <t>Optum</t>
+  </si>
+  <si>
+    <t>Career India(Mechanical Only)</t>
+  </si>
+  <si>
+    <t>Technip India Ltd.(EE,ME,CIE,CE)</t>
+  </si>
+  <si>
+    <t>Samsung E&amp;A India (EE,ME,CE)</t>
   </si>
 </sst>
 </file>
@@ -338,12 +404,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -561,7 +630,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="25.88"/>
+    <col customWidth="1" min="2" max="2" width="36.38"/>
     <col customWidth="1" min="3" max="3" width="29.88"/>
     <col customWidth="1" min="4" max="4" width="17.5"/>
     <col customWidth="1" min="5" max="5" width="25.63"/>
@@ -590,16 +659,19 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1">
         <v>10.0</v>
@@ -610,13 +682,13 @@
     </row>
     <row r="3">
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1">
         <v>33.0</v>
@@ -627,13 +699,13 @@
     </row>
     <row r="4">
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1">
         <v>30.0</v>
@@ -644,13 +716,13 @@
     </row>
     <row r="5">
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1">
         <v>4.0</v>
@@ -661,13 +733,13 @@
     </row>
     <row r="6">
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1">
         <v>3.0</v>
@@ -678,13 +750,13 @@
     </row>
     <row r="7">
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1">
         <v>10.0</v>
@@ -695,12 +767,14 @@
     </row>
     <row r="8">
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E8" s="1">
         <v>0.0</v>
       </c>
@@ -710,13 +784,13 @@
     </row>
     <row r="9">
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E9" s="1">
         <v>5.0</v>
@@ -727,13 +801,13 @@
     </row>
     <row r="10">
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1">
         <v>2.0</v>
@@ -744,10 +818,10 @@
     </row>
     <row r="11">
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1">
         <v>2.0</v>
@@ -758,10 +832,10 @@
     </row>
     <row r="12">
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="1">
         <v>3.0</v>
@@ -772,10 +846,10 @@
     </row>
     <row r="13">
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1">
         <v>2.0</v>
@@ -786,10 +860,10 @@
     </row>
     <row r="14">
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" s="1">
         <v>1.0</v>
@@ -800,10 +874,10 @@
     </row>
     <row r="15">
       <c r="C15" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" s="1">
         <v>3.0</v>
@@ -814,10 +888,10 @@
     </row>
     <row r="16">
       <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" s="1">
         <v>1.0</v>
@@ -828,10 +902,10 @@
     </row>
     <row r="17">
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" s="1">
         <v>3.0</v>
@@ -842,10 +916,10 @@
     </row>
     <row r="18">
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18" s="1">
         <v>2.0</v>
@@ -856,10 +930,10 @@
     </row>
     <row r="19">
       <c r="C19" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E19" s="1">
         <v>5.0</v>
@@ -870,10 +944,10 @@
     </row>
     <row r="20">
       <c r="C20" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E20" s="1">
         <v>3.0</v>
@@ -884,10 +958,10 @@
     </row>
     <row r="21">
       <c r="C21" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E21" s="1">
         <v>2.0</v>
@@ -898,10 +972,10 @@
     </row>
     <row r="22">
       <c r="C22" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E22" s="1">
         <v>2.0</v>
@@ -912,10 +986,10 @@
     </row>
     <row r="23">
       <c r="C23" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E23" s="1">
         <v>1.0</v>
@@ -926,10 +1000,10 @@
     </row>
     <row r="24">
       <c r="C24" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E24" s="1">
         <v>1.0</v>
@@ -940,72 +1014,72 @@
     </row>
     <row r="25">
       <c r="B25" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E25" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="F25" s="1">
-        <v>20.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1.0</v>
       </c>
       <c r="F26" s="1">
-        <v>17.3</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="27">
+      <c r="B27" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="C27" s="1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F27" s="1">
         <v>17.3</v>
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="1" t="s">
-        <v>41</v>
+      <c r="C28" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F28" s="1">
-        <v>14.0</v>
+        <v>17.3</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>44</v>
+        <v>13</v>
+      </c>
+      <c r="F29" s="1">
+        <v>14.0</v>
       </c>
     </row>
     <row r="30">
@@ -1016,182 +1090,249 @@
         <v>46</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E30" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="F30" s="1">
-        <v>17.91</v>
+        <v>5.0</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="1">
+        <v>2.0</v>
       </c>
       <c r="F31" s="1">
-        <v>14.0</v>
+        <v>17.91</v>
       </c>
     </row>
     <row r="32">
+      <c r="B32" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="C32" s="1" t="s">
-        <v>49</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="1"/>
       <c r="F32" s="1">
-        <v>14.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>14.0</v>
       </c>
     </row>
     <row r="34">
-      <c r="B34" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="C34" s="1" t="s">
-        <v>20</v>
+        <v>54</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E34" s="1">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="F34" s="1">
-        <v>17.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" s="1">
-        <v>25.0</v>
+        <v>22</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>55</v>
+        <v>22</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>17.0</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F37" s="1">
-        <v>19.5</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F38" s="1">
-        <v>14.75</v>
+        <v>22</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F39" s="1">
-        <v>15.0</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F40" s="1">
-        <v>6.0</v>
+        <v>14.75</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F41" s="1">
-        <v>6.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>20</v>
+        <v>64</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F42" s="1">
-        <v>14.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="1">
+        <v>6.0</v>
       </c>
     </row>
     <row r="44">
+      <c r="B44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="1">
+        <v>4.0</v>
+      </c>
       <c r="F44" s="1">
-        <v>0.75</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F45" s="1">
-        <v>0.75</v>
+        <v>22</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="46">
-      <c r="C46" s="1" t="s">
-        <v>66</v>
+      <c r="D46" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F46" s="1">
         <v>0.75</v>
       </c>
     </row>
     <row r="47">
+      <c r="B47" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="C47" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E47" s="1">
-        <v>6.0</v>
+        <v>70</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F47" s="1">
         <v>0.75</v>
@@ -1199,233 +1340,453 @@
     </row>
     <row r="48">
       <c r="C48" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E48" s="1">
+        <v>71</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="C49" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="1">
         <v>6.0</v>
       </c>
-      <c r="F48" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="B49" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="F49" s="1">
-        <v>9.0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="50">
       <c r="C50" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" s="1">
+        <v>6.0</v>
       </c>
       <c r="F50" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="C52" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="1">
         <v>7.0</v>
       </c>
     </row>
-    <row r="51">
-      <c r="C51" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F51" s="1">
+    <row r="53">
+      <c r="C53" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="1">
         <v>3.3</v>
       </c>
     </row>
-    <row r="52">
-      <c r="B52" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F52" s="1">
-        <v>14.0</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="B53" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F53" s="1">
-        <v>11.0</v>
-      </c>
-    </row>
     <row r="54">
+      <c r="B54" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="C54" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F54" s="1">
-        <v>11.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>78</v>
+        <v>54</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="F55" s="1">
+        <v>11.0</v>
       </c>
     </row>
     <row r="56">
-      <c r="B56" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="C56" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="1">
+        <v>1.0</v>
       </c>
       <c r="F56" s="1">
-        <v>45.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F57" s="1">
-        <v>22.0</v>
+        <v>22</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="1">
+        <v>45.0</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F59" s="1">
-        <v>18.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F60" s="1">
-        <v>7.0</v>
+        <v>88</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E61" s="1">
-        <v>24.0</v>
+      <c r="D61" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F61" s="1">
-        <v>13.65</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>49</v>
+        <v>91</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F62" s="1">
-        <v>13.38</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63" s="1">
+        <v>24.0</v>
       </c>
       <c r="F63" s="1">
-        <v>15.75</v>
+        <v>13.65</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>20</v>
+        <v>54</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F64" s="1">
-        <v>34.0</v>
+        <v>13.38</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F65" s="1">
-        <v>13.0</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="1"/>
     </row>
     <row r="66">
       <c r="B66" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F66" s="1">
-        <v>11.0</v>
+        <v>15.75</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F67" s="1">
-        <v>12.2</v>
+        <v>34.0</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>96</v>
+        <v>22</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F68" s="1">
-        <v>7.5</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>88</v>
+        <v>99</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F69" s="1">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F70" s="1">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F71" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F72" s="1">
         <v>8.1</v>
       </c>
     </row>
-    <row r="70">
-      <c r="E70" s="1"/>
+    <row r="73">
+      <c r="B73" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E73" s="1"/>
+    </row>
+    <row r="74">
+      <c r="B74" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1">
+        <v>18.4</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F80" s="1">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="B82" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F82" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F83" s="1">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update list with companies in september, updated format.
</commit_message>
<xml_diff>
--- a/Thapar BE_B Tech 2025 Placement Data.xlsx
+++ b/Thapar BE_B Tech 2025 Placement Data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="329">
   <si>
     <t>S No.</t>
   </si>
@@ -31,10 +31,19 @@
     <t>CTC(LPA)</t>
   </si>
   <si>
+    <t>Stipend</t>
+  </si>
+  <si>
     <t>Location</t>
   </si>
   <si>
-    <t>CG Cut</t>
+    <t>Eligibility</t>
+  </si>
+  <si>
+    <t>Branches</t>
+  </si>
+  <si>
+    <t>Special Comments</t>
   </si>
   <si>
     <t>JP Morgan</t>
@@ -46,6 +55,21 @@
     <t>April</t>
   </si>
   <si>
+    <t>19.75(13 base)</t>
+  </si>
+  <si>
+    <t>75k/mo</t>
+  </si>
+  <si>
+    <t>Mumabi/Hyderabad/Bangalore</t>
+  </si>
+  <si>
+    <t>8.5CG+</t>
+  </si>
+  <si>
+    <t>CS-All Branches ENC</t>
+  </si>
+  <si>
     <t>Blackrock</t>
   </si>
   <si>
@@ -55,6 +79,18 @@
     <t>August</t>
   </si>
   <si>
+    <t>50k/mo</t>
+  </si>
+  <si>
+    <t>NCR/ All over India</t>
+  </si>
+  <si>
+    <t>6CG+</t>
+  </si>
+  <si>
+    <t>CS-All Branches ENC/ECE/EE/EIC/EEC</t>
+  </si>
+  <si>
     <t>Data And Software Engineering</t>
   </si>
   <si>
@@ -82,12 +118,36 @@
     <t>SDE</t>
   </si>
   <si>
+    <t>28(21.9 base</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>No Criteria</t>
+  </si>
+  <si>
+    <t>All Branches</t>
+  </si>
+  <si>
     <t>Bain</t>
   </si>
   <si>
     <t>Communication</t>
   </si>
   <si>
+    <t>40k/mo</t>
+  </si>
+  <si>
+    <t>Gurugram/Bangalore</t>
+  </si>
+  <si>
+    <t>CS-All branches EE/EIC/ENC/ECE/EEC/Mech/BME</t>
+  </si>
+  <si>
     <t>Financial Services</t>
   </si>
   <si>
@@ -133,7 +193,16 @@
     <t>Arista(Through ACE Certification Program)</t>
   </si>
   <si>
-    <t>-</t>
+    <t>13(10 base)</t>
+  </si>
+  <si>
+    <t>25k/mo</t>
+  </si>
+  <si>
+    <t>Noida/Bangalore/Hyderabad/Pune</t>
+  </si>
+  <si>
+    <t>Dual Degree</t>
   </si>
   <si>
     <t>Cloudera</t>
@@ -145,9 +214,6 @@
     <t>Technical Analyst</t>
   </si>
   <si>
-    <t>Infinera</t>
-  </si>
-  <si>
     <t>AlgoSec</t>
   </si>
   <si>
@@ -157,12 +223,27 @@
     <t>18-20</t>
   </si>
   <si>
+    <t>Gurugram</t>
+  </si>
+  <si>
+    <t>CS-All Branches</t>
+  </si>
+  <si>
     <t>American Express</t>
   </si>
   <si>
     <t>AI Product Analyst</t>
   </si>
   <si>
+    <t>17.91(13.87 base)</t>
+  </si>
+  <si>
+    <t>1lac/mo</t>
+  </si>
+  <si>
+    <t>7CG+</t>
+  </si>
+  <si>
     <t>IBM</t>
   </si>
   <si>
@@ -175,21 +256,57 @@
     <t xml:space="preserve">SWE </t>
   </si>
   <si>
+    <t>14(13 base)</t>
+  </si>
+  <si>
+    <t>30k/mo</t>
+  </si>
+  <si>
+    <t>Bangalore(Domlur)</t>
+  </si>
+  <si>
+    <t>6.5CG+</t>
+  </si>
+  <si>
+    <t>CS-All Branches ECE/ENC/EEC</t>
+  </si>
+  <si>
     <t>Business Analyst</t>
   </si>
   <si>
     <t>Zhealthehr</t>
   </si>
   <si>
-    <t>35(14 Stock)</t>
+    <t>35(13 base 14 Stock)</t>
+  </si>
+  <si>
+    <t>27k/mo</t>
+  </si>
+  <si>
+    <t>Gurugram/Noida</t>
+  </si>
+  <si>
+    <t>8CG+</t>
   </si>
   <si>
     <t xml:space="preserve">Fastenal </t>
   </si>
   <si>
+    <t>17(15 base)</t>
+  </si>
+  <si>
+    <t>45k/mo</t>
+  </si>
+  <si>
+    <t>CS-All Branches ECE/ENC/EEC/EIC/EE</t>
+  </si>
+  <si>
     <t>Wayfair</t>
   </si>
   <si>
+    <t>25(23 base)</t>
+  </si>
+  <si>
     <t>GamesKraft</t>
   </si>
   <si>
@@ -199,15 +316,42 @@
     <t>Oracle</t>
   </si>
   <si>
+    <t>19.5(14.5 base)</t>
+  </si>
+  <si>
+    <t>Not given</t>
+  </si>
+  <si>
+    <t>CS- All branhces ENC/ECE/EEC/EIC/EE/</t>
+  </si>
+  <si>
     <t>Airtel</t>
   </si>
   <si>
+    <t>14.75(12.75 base)</t>
+  </si>
+  <si>
+    <t>Pan India</t>
+  </si>
+  <si>
     <t>Deutsche Telekom</t>
   </si>
   <si>
+    <t>15(13 base)</t>
+  </si>
+  <si>
+    <t>Gurgaon</t>
+  </si>
+  <si>
+    <t>CS- All branhces ENC/ECE/EEC</t>
+  </si>
+  <si>
     <t>Siemens SPEL</t>
   </si>
   <si>
+    <t>CS-EE/ECE/EIC/Mech.</t>
+  </si>
+  <si>
     <t>Siemens Ltd.</t>
   </si>
   <si>
@@ -217,7 +361,7 @@
     <t>Apple(Intern-Only)</t>
   </si>
   <si>
-    <t>0.9 + 0.83(reloc)</t>
+    <t>90k/mo +10k/mo + 80k(Reloc)</t>
   </si>
   <si>
     <t xml:space="preserve">JP Morgan </t>
@@ -286,9 +430,6 @@
     <t>Warner Bros</t>
   </si>
   <si>
-    <t>SRF Ltd.</t>
-  </si>
-  <si>
     <t>ZS</t>
   </si>
   <si>
@@ -304,18 +445,54 @@
     <t>Hardware</t>
   </si>
   <si>
+    <t>45K/mo</t>
+  </si>
+  <si>
+    <t>CS-All branches ECE/ENC</t>
+  </si>
+  <si>
     <t>Meesho</t>
   </si>
   <si>
+    <t>34(20 base)</t>
+  </si>
+  <si>
+    <t>No CG Criteria</t>
+  </si>
+  <si>
+    <t>CS- All branches ENC/ECE/EIC/EE/EEC</t>
+  </si>
+  <si>
     <t>British Telecom</t>
   </si>
   <si>
+    <t>17(13 base)</t>
+  </si>
+  <si>
+    <t>60k/mo</t>
+  </si>
+  <si>
+    <t>CS- ALL branches ENC/ECE</t>
+  </si>
+  <si>
     <t>Loreal Paris</t>
   </si>
   <si>
+    <t>20k/mo</t>
+  </si>
+  <si>
+    <t>Baddi(HImachal Pradesh)</t>
+  </si>
+  <si>
+    <t>Chem/EE/EIC/EEC/ME</t>
+  </si>
+  <si>
     <t>Viscadia</t>
   </si>
   <si>
+    <t>CS-All branches ECE/ENC/EE/EIC/EEC</t>
+  </si>
+  <si>
     <t>Volvo</t>
   </si>
   <si>
@@ -331,7 +508,25 @@
     <t>Verizon</t>
   </si>
   <si>
+    <t>9.74(7 base)</t>
+  </si>
+  <si>
+    <t>Chennai/Hyderbad/Bangalore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CS-All branches </t>
+  </si>
+  <si>
     <t>Amadeus Labs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graduate Engineer </t>
+  </si>
+  <si>
+    <t>7.5CG+</t>
+  </si>
+  <si>
+    <t>CS-All branches ENC/ECE/EEC/EE</t>
   </si>
   <si>
     <t>Honda</t>
@@ -358,26 +553,467 @@
     </r>
   </si>
   <si>
+    <t>18.4(16 base)</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>CS-All branches</t>
+  </si>
+  <si>
+    <t>1Lakh payment if u resign after intern</t>
+  </si>
+  <si>
     <t>GEP Worldwide</t>
   </si>
   <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>17(16 base)</t>
+  </si>
+  <si>
+    <t>Hyderabad/Mumbai</t>
+  </si>
+  <si>
     <t>Optum</t>
   </si>
   <si>
-    <t>Career India(Mechanical Only)</t>
-  </si>
-  <si>
-    <t>Technip India Ltd.(EE,ME,CIE,CE)</t>
-  </si>
-  <si>
-    <t>Samsung E&amp;A India (EE,ME,CE)</t>
+    <t>18.5(15.5 base)</t>
+  </si>
+  <si>
+    <t>Gurgaon/Hyderbad</t>
+  </si>
+  <si>
+    <t>CS-All branches ENC/EEC/ECE/EE/EIC</t>
+  </si>
+  <si>
+    <t>Career India</t>
+  </si>
+  <si>
+    <t>8.5(7.5 base)</t>
+  </si>
+  <si>
+    <t>Mechanical</t>
+  </si>
+  <si>
+    <t>Technip India Ltd</t>
+  </si>
+  <si>
+    <t>EE/ME/CIE/CE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samsung E&amp;A India </t>
+  </si>
+  <si>
+    <t>EE/ME/CE</t>
+  </si>
+  <si>
+    <t>Locofast</t>
+  </si>
+  <si>
+    <t>10(9 base)</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
+    <t>7 Cg+, 80% in 12th</t>
+  </si>
+  <si>
+    <t>CS- All branches</t>
+  </si>
+  <si>
+    <t>UKG</t>
+  </si>
+  <si>
+    <t>21(15.5 base)</t>
+  </si>
+  <si>
+    <t>Noida</t>
+  </si>
+  <si>
+    <t>CS-All branches ENC/ECE</t>
+  </si>
+  <si>
+    <t>Siemens EDA Pvt. Ltd.</t>
+  </si>
+  <si>
+    <t>24(16.5 base)</t>
+  </si>
+  <si>
+    <t>Noida/Bangalore/Kolkata</t>
+  </si>
+  <si>
+    <t>CS- All branches ENC/EEC/EIC/ECE/EE</t>
+  </si>
+  <si>
+    <t>SDE(OS Role)</t>
+  </si>
+  <si>
+    <t>Analog</t>
+  </si>
+  <si>
+    <t>Digital</t>
+  </si>
+  <si>
+    <t>Infinera</t>
+  </si>
+  <si>
+    <t>14(13.3 base)</t>
+  </si>
+  <si>
+    <t>ECE/ENC</t>
+  </si>
+  <si>
+    <t>Zavya</t>
+  </si>
+  <si>
+    <t>20-25k/mo</t>
+  </si>
+  <si>
+    <t>All Branches(Except Civil)</t>
+  </si>
+  <si>
+    <t>Addverb</t>
+  </si>
+  <si>
+    <t>GET-Software</t>
+  </si>
+  <si>
+    <t>CS-All branches/EE/EIC.EC.ENC/EEC</t>
+  </si>
+  <si>
+    <t>GET- Mobile Robotics</t>
+  </si>
+  <si>
+    <t>CS-All branches/EE/EIC.EC.ENC/EEC/Mech.</t>
+  </si>
+  <si>
+    <t>FNZ</t>
+  </si>
+  <si>
+    <t>Junior Analyst Developer</t>
+  </si>
+  <si>
+    <t>8.4CG+</t>
+  </si>
+  <si>
+    <t>CS- All Branches ECE/ENC/EEC</t>
+  </si>
+  <si>
+    <t>Junior Analyst Developer FNZ Studio</t>
+  </si>
+  <si>
+    <t>Junior Analyst Tester</t>
+  </si>
+  <si>
+    <t>BE- All Streams</t>
+  </si>
+  <si>
+    <t>WTW India</t>
+  </si>
+  <si>
+    <t>Lumber</t>
+  </si>
+  <si>
+    <t>Digital X Force</t>
+  </si>
+  <si>
+    <t>Cyber Security Intern</t>
+  </si>
+  <si>
+    <t>15k/mo</t>
+  </si>
+  <si>
+    <t>Mohali/Chandigrah/Delhi</t>
+  </si>
+  <si>
+    <t>CS- All branches ENC/EEC</t>
+  </si>
+  <si>
+    <t>Barco</t>
+  </si>
+  <si>
+    <t>18(15 base)</t>
+  </si>
+  <si>
+    <t>Shared later</t>
+  </si>
+  <si>
+    <t>Morphle Labs</t>
+  </si>
+  <si>
+    <t>Mech</t>
+  </si>
+  <si>
+    <t>ZScaler</t>
+  </si>
+  <si>
+    <t>shared later</t>
+  </si>
+  <si>
+    <t>Bangalore/Pune/Mohali/Hyderabad</t>
+  </si>
+  <si>
+    <t>CSE/COE/EE/EIC/ECE/ENC</t>
+  </si>
+  <si>
+    <t>Stone Wein Systems</t>
+  </si>
+  <si>
+    <t>11(9 base)</t>
+  </si>
+  <si>
+    <t>Chandigarh/Pune</t>
+  </si>
+  <si>
+    <t>CS- All branches ENC</t>
+  </si>
+  <si>
+    <t>2  lakh if u resign before 1 year</t>
+  </si>
+  <si>
+    <t>HSBC</t>
+  </si>
+  <si>
+    <t>9(CTC mentioned only)</t>
+  </si>
+  <si>
+    <t>Pune/Hyderabad/Bengaluru</t>
+  </si>
+  <si>
+    <t>CS- All Branches</t>
+  </si>
+  <si>
+    <t>Advantage Club</t>
+  </si>
+  <si>
+    <t>Backend Developer</t>
+  </si>
+  <si>
+    <t>14(10 base + 4 ESOPs)</t>
+  </si>
+  <si>
+    <t>6.50CG+</t>
+  </si>
+  <si>
+    <t>Product Manager</t>
+  </si>
+  <si>
+    <t>QA &amp; Testing Engineer</t>
+  </si>
+  <si>
+    <t>12(8 base + 4 ESOPs)</t>
+  </si>
+  <si>
+    <t>Arista Networks</t>
+  </si>
+  <si>
+    <t>Software Tester</t>
+  </si>
+  <si>
+    <t>22.5( base 15)</t>
+  </si>
+  <si>
+    <t>65k/mo + 50k reloc</t>
+  </si>
+  <si>
+    <t>Bengaluru</t>
+  </si>
+  <si>
+    <t>7.50CG+</t>
+  </si>
+  <si>
+    <t>21.1(base 14)</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>Airtel YTL Digital</t>
+  </si>
+  <si>
+    <t>Young Technical Leader</t>
+  </si>
+  <si>
+    <t>Accenture</t>
+  </si>
+  <si>
+    <t>Advance Application Enginnering Analyst</t>
+  </si>
+  <si>
+    <t>10.9( base 9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Branches </t>
+  </si>
+  <si>
+    <t>Commvault Systems</t>
+  </si>
+  <si>
+    <t>Software Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 base + 19k USD RSUs + 1.5 JB </t>
+  </si>
+  <si>
+    <t>CS-All branches /ENC</t>
+  </si>
+  <si>
+    <t>Software Quality</t>
+  </si>
+  <si>
+    <t>Development(CPP Or Java)</t>
+  </si>
+  <si>
+    <t>Testing(Python)</t>
+  </si>
+  <si>
+    <t>Nvidia</t>
+  </si>
+  <si>
+    <t>GPU Architecture Team</t>
+  </si>
+  <si>
+    <t>Hyderabad/Pune/Bangalore</t>
+  </si>
+  <si>
+    <t>7.8CG+</t>
+  </si>
+  <si>
+    <t>CS-All bramches/EE/EIC/ECE/ENC/EEC</t>
+  </si>
+  <si>
+    <t>Infra Team</t>
+  </si>
+  <si>
+    <t>VLSI Team</t>
+  </si>
+  <si>
+    <t>CPU Design And Verification Team</t>
+  </si>
+  <si>
+    <t>SoC TEGRA Design &amp; Verification</t>
+  </si>
+  <si>
+    <t>GPU ASIC Design Team</t>
+  </si>
+  <si>
+    <t>Oyo rooms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASDE </t>
+  </si>
+  <si>
+    <t>CS-All branches/ENC/EEC/EC/CIVIL/EE/EIC/MECH/MECHA</t>
+  </si>
+  <si>
+    <t>MG Motor India</t>
+  </si>
+  <si>
+    <t>Gurugram/Halol/Mumbai/Bamgalore</t>
+  </si>
+  <si>
+    <t>EE/EIC/ECE/ENC/EEC/MECH/MECHA</t>
+  </si>
+  <si>
+    <t>Atkins Realis</t>
+  </si>
+  <si>
+    <t>CS-All branches/CIE/ME/EE/ECE/Chem./EIC</t>
+  </si>
+  <si>
+    <t>Evalueserve</t>
+  </si>
+  <si>
+    <t>Customer Insights And Data Analytics</t>
+  </si>
+  <si>
+    <t>Varroc Group</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>11.5(9 base)</t>
+  </si>
+  <si>
+    <t>MECHA</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Wireless Technology And Ecosystems</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>90k/mo +10k/mo + 73k(reloc)</t>
+  </si>
+  <si>
+    <t>CS- All branches/EE/EIC/ENC/ECE/EEC</t>
+  </si>
+  <si>
+    <t>SRF Ltd.</t>
+  </si>
+  <si>
+    <t>Chem</t>
+  </si>
+  <si>
+    <t>Techno Electric &amp; Engineering Co Ltd.</t>
+  </si>
+  <si>
+    <t>Civil/EE</t>
+  </si>
+  <si>
+    <t>Midea India Pvt. Ltd.</t>
+  </si>
+  <si>
+    <t>0k/mo(unpaid intern)</t>
+  </si>
+  <si>
+    <t>Ahmednagar</t>
+  </si>
+  <si>
+    <t>EE/ECE/MECH/MECHA</t>
+  </si>
+  <si>
+    <t>NuvertOS</t>
+  </si>
+  <si>
+    <t>9CG+</t>
+  </si>
+  <si>
+    <t>NXP Semiconductors</t>
+  </si>
+  <si>
+    <t>Digital Design</t>
+  </si>
+  <si>
+    <t>42.5k/mo</t>
+  </si>
+  <si>
+    <t>Noida/Bangalore/Pune/Hyderabad</t>
+  </si>
+  <si>
+    <t>ECE</t>
+  </si>
+  <si>
+    <t>Analog &amp; Software Engineer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m-d"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -389,13 +1025,23 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -404,7 +1050,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -412,6 +1058,12 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -631,10 +1283,15 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="36.38"/>
-    <col customWidth="1" min="3" max="3" width="29.88"/>
+    <col customWidth="1" min="3" max="3" width="33.13"/>
     <col customWidth="1" min="4" max="4" width="17.5"/>
     <col customWidth="1" min="5" max="5" width="25.63"/>
-    <col customWidth="1" min="6" max="6" width="19.38"/>
+    <col customWidth="1" min="6" max="6" width="37.38"/>
+    <col customWidth="1" min="7" max="7" width="26.25"/>
+    <col customWidth="1" min="8" max="8" width="32.13"/>
+    <col customWidth="1" min="9" max="9" width="23.88"/>
+    <col customWidth="1" min="10" max="10" width="48.13"/>
+    <col customWidth="1" min="11" max="11" width="30.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -662,33 +1319,54 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1">
         <v>10.0</v>
       </c>
-      <c r="F2" s="1">
-        <v>19.75</v>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1">
         <v>33.0</v>
@@ -696,16 +1374,28 @@
       <c r="F3" s="1">
         <v>18.0</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1">
         <v>30.0</v>
@@ -713,16 +1403,28 @@
       <c r="F4" s="1">
         <v>18.0</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1">
         <v>4.0</v>
@@ -730,16 +1432,28 @@
       <c r="F5" s="1">
         <v>18.0</v>
       </c>
+      <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1">
         <v>3.0</v>
@@ -747,16 +1461,28 @@
       <c r="F6" s="1">
         <v>22.0</v>
       </c>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1">
         <v>10.0</v>
@@ -764,19 +1490,31 @@
       <c r="F7" s="1">
         <v>22.0</v>
       </c>
+      <c r="G7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="F8" s="1">
         <v>9.5</v>
@@ -784,30 +1522,42 @@
     </row>
     <row r="9">
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1">
         <v>5.0</v>
       </c>
-      <c r="F9" s="1">
-        <v>28.0</v>
+      <c r="F9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E10" s="1">
         <v>2.0</v>
@@ -815,13 +1565,28 @@
       <c r="F10" s="1">
         <v>14.0</v>
       </c>
+      <c r="G10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="11">
+      <c r="B11" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E11" s="1">
         <v>2.0</v>
@@ -829,13 +1594,28 @@
       <c r="F11" s="1">
         <v>14.0</v>
       </c>
+      <c r="G11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="12">
+      <c r="B12" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E12" s="1">
         <v>3.0</v>
@@ -843,13 +1623,28 @@
       <c r="F12" s="1">
         <v>14.0</v>
       </c>
+      <c r="G12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="13">
+      <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E13" s="1">
         <v>2.0</v>
@@ -857,13 +1652,28 @@
       <c r="F13" s="1">
         <v>14.0</v>
       </c>
+      <c r="G13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14">
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E14" s="1">
         <v>1.0</v>
@@ -871,13 +1681,28 @@
       <c r="F14" s="1">
         <v>14.0</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="15">
+      <c r="B15" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E15" s="1">
         <v>3.0</v>
@@ -885,13 +1710,28 @@
       <c r="F15" s="1">
         <v>14.0</v>
       </c>
+      <c r="G15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16">
+      <c r="B16" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E16" s="1">
         <v>1.0</v>
@@ -899,13 +1739,28 @@
       <c r="F16" s="1">
         <v>14.0</v>
       </c>
+      <c r="G16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="17">
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E17" s="1">
         <v>3.0</v>
@@ -913,13 +1768,28 @@
       <c r="F17" s="1">
         <v>14.0</v>
       </c>
+      <c r="G17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="18">
+      <c r="B18" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="E18" s="1">
         <v>2.0</v>
@@ -927,13 +1797,28 @@
       <c r="F18" s="1">
         <v>14.0</v>
       </c>
+      <c r="G18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="19">
+      <c r="B19" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E19" s="1">
         <v>5.0</v>
@@ -941,13 +1826,28 @@
       <c r="F19" s="1">
         <v>14.0</v>
       </c>
+      <c r="G19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="20">
+      <c r="B20" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C20" s="1" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E20" s="1">
         <v>3.0</v>
@@ -955,13 +1855,28 @@
       <c r="F20" s="1">
         <v>14.0</v>
       </c>
+      <c r="G20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="21">
+      <c r="B21" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C21" s="1" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E21" s="1">
         <v>2.0</v>
@@ -969,13 +1884,28 @@
       <c r="F21" s="1">
         <v>14.0</v>
       </c>
+      <c r="G21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="22">
+      <c r="B22" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C22" s="1" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E22" s="1">
         <v>2.0</v>
@@ -983,13 +1913,28 @@
       <c r="F22" s="1">
         <v>14.0</v>
       </c>
+      <c r="G22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="23">
+      <c r="B23" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C23" s="1" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E23" s="1">
         <v>1.0</v>
@@ -997,13 +1942,28 @@
       <c r="F23" s="1">
         <v>14.0</v>
       </c>
+      <c r="G23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="24">
+      <c r="B24" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="C24" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E24" s="1">
         <v>1.0</v>
@@ -1011,33 +1971,57 @@
       <c r="F24" s="1">
         <v>14.0</v>
       </c>
+      <c r="G24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="1" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E25" s="1">
         <v>4.0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>40</v>
+        <v>60</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" s="1" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E26" s="1">
         <v>1.0</v>
@@ -1048,24 +2032,27 @@
     </row>
     <row r="27">
       <c r="B27" s="1" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F27" s="1">
         <v>17.3</v>
       </c>
     </row>
     <row r="28">
+      <c r="B28" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="C28" s="1" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F28" s="1">
         <v>17.3</v>
@@ -1073,719 +2060,2326 @@
     </row>
     <row r="29">
       <c r="B29" s="1" t="s">
-        <v>44</v>
+        <v>67</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="1">
-        <v>14.0</v>
+        <v>21</v>
+      </c>
+      <c r="E29" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" s="1" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E30" s="1">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>47</v>
+        <v>74</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" s="1" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" s="1">
-        <v>2.0</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E31" s="1"/>
       <c r="F31" s="1">
-        <v>17.91</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" s="1" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1">
-        <v>12.0</v>
+        <v>21</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" s="1" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E33" s="1">
         <v>1.0</v>
       </c>
-      <c r="F33" s="1">
-        <v>14.0</v>
+      <c r="F33" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="34">
+      <c r="B34" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="C34" s="1" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="F34" s="1">
-        <v>14.0</v>
+        <v>21</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" s="1" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="E35" s="1">
+        <v>5.0</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>56</v>
+        <v>93</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" s="1" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="F36" s="1">
-        <v>17.0</v>
+        <v>21</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" s="1" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="1">
-        <v>25.0</v>
+        <v>21</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" s="1" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>60</v>
+      <c r="H38" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" s="1" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" s="1">
-        <v>19.5</v>
+        <v>21</v>
+      </c>
+      <c r="E39" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" s="1" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" s="1">
-        <v>14.75</v>
+        <v>21</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>22</v>
+        <v>111</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F41" s="1">
-        <v>15.0</v>
+        <v>6.0</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" s="1" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F42" s="1">
         <v>6.0</v>
       </c>
+      <c r="G42" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="43">
       <c r="B43" s="1" t="s">
-        <v>65</v>
+        <v>114</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="E43" s="1">
+        <v>4.0</v>
       </c>
       <c r="F43" s="1">
-        <v>6.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" s="1" t="s">
-        <v>66</v>
+        <v>115</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E44" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="F44" s="1">
-        <v>14.0</v>
+        <v>16.0</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" s="1" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>22</v>
+        <v>118</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>68</v>
+        <v>21</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="46">
+      <c r="B46" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="D46" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F46" s="1">
-        <v>0.75</v>
+        <v>21</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" s="1" t="s">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F47" s="1">
-        <v>0.75</v>
+        <v>21</v>
+      </c>
+      <c r="E47" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="48">
+      <c r="B48" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="C48" s="1" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F48" s="1">
-        <v>0.75</v>
+        <v>21</v>
+      </c>
+      <c r="E48" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="49">
+      <c r="B49" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="C49" s="1" t="s">
-        <v>72</v>
+        <v>123</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E49" s="1">
-        <v>6.0</v>
+        <v>21</v>
       </c>
       <c r="F49" s="1">
-        <v>0.75</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="50">
+      <c r="B50" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="C50" s="1" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E50" s="1">
-        <v>6.0</v>
+        <v>21</v>
       </c>
       <c r="F50" s="1">
-        <v>0.5</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" s="1" t="s">
-        <v>74</v>
+        <v>122</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F51" s="1">
-        <v>9.0</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="52">
+      <c r="B52" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="C52" s="1" t="s">
-        <v>76</v>
+        <v>127</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F52" s="1">
-        <v>7.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="53">
+      <c r="B53" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="C53" s="1" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="E53" s="1">
+        <v>6.0</v>
       </c>
       <c r="F53" s="1">
-        <v>3.3</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" s="1" t="s">
-        <v>78</v>
+        <v>128</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>79</v>
+        <v>129</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="E54" s="1">
+        <v>1.0</v>
       </c>
       <c r="F54" s="1">
-        <v>14.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" s="1" t="s">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E55" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="F55" s="1">
-        <v>11.0</v>
+        <v>21</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="56">
+      <c r="B56" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="C56" s="1" t="s">
-        <v>81</v>
+        <v>133</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E56" s="1">
-        <v>1.0</v>
+        <v>21</v>
       </c>
       <c r="F56" s="1">
-        <v>11.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" s="1" t="s">
-        <v>82</v>
+        <v>134</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>22</v>
+        <v>135</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>83</v>
+        <v>21</v>
+      </c>
+      <c r="F57" s="1">
+        <v>22.0</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" s="1" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F58" s="1">
-        <v>45.0</v>
+        <v>21</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" s="1" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F59" s="1">
-        <v>22.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" s="1" t="s">
-        <v>88</v>
+        <v>139</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>22</v>
+        <v>140</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>89</v>
+        <v>21</v>
+      </c>
+      <c r="E60" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="F60" s="1">
+        <v>13.65</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" s="1" t="s">
-        <v>90</v>
+        <v>141</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F61" s="1">
-        <v>18.0</v>
+        <v>13.38</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" s="1" t="s">
-        <v>91</v>
+        <v>142</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F62" s="1">
-        <v>7.0</v>
+        <v>15.75</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" s="1" t="s">
-        <v>92</v>
+        <v>142</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E63" s="1">
-        <v>24.0</v>
+        <v>21</v>
       </c>
       <c r="F63" s="1">
-        <v>13.65</v>
+        <v>15.75</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E64" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F64" s="1">
-        <v>13.38</v>
+      <c r="H64" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" s="1" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>96</v>
+        <v>34</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F65" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="E65" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="66">
       <c r="B66" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>22</v>
+        <v>154</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F66" s="1">
-        <v>15.75</v>
+        <v>11.0</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" s="1" t="s">
-        <v>97</v>
+        <v>158</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F67" s="1">
+        <v>12.2</v>
+      </c>
+      <c r="G67" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F67" s="1">
-        <v>34.0</v>
+      <c r="I67" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" s="1" t="s">
-        <v>98</v>
+        <v>160</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>22</v>
+        <v>161</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F68" s="1">
-        <v>13.0</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" s="1" t="s">
-        <v>99</v>
+        <v>162</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="E69" s="1">
+        <v>39.0</v>
       </c>
       <c r="F69" s="1">
-        <v>11.0</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="70">
       <c r="B70" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>22</v>
+        <v>163</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E70" s="1"/>
       <c r="F70" s="1">
-        <v>12.2</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>102</v>
+        <v>164</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F71" s="1">
-        <v>7.5</v>
+        <v>21</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" s="1" t="s">
-        <v>103</v>
+        <v>168</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>93</v>
+        <v>169</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="E72" s="1">
+        <v>18.0</v>
       </c>
       <c r="F72" s="1">
-        <v>8.1</v>
+        <v>12.62</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" s="1" t="s">
-        <v>104</v>
+        <v>172</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E73" s="1"/>
+        <v>21</v>
+      </c>
     </row>
     <row r="74">
       <c r="B74" s="1" t="s">
-        <v>78</v>
+        <v>173</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1">
+        <v>13.2</v>
       </c>
     </row>
     <row r="75">
       <c r="B75" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>13</v>
+        <v>175</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E75" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="76">
       <c r="B76" s="1" t="s">
-        <v>106</v>
+        <v>182</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>13</v>
+        <v>183</v>
+      </c>
+      <c r="E76" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>13</v>
+        <v>186</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E77" s="1">
+        <v>67.0</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="78">
       <c r="B78" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>109</v>
+        <v>190</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1">
-        <v>13.2</v>
+        <v>183</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="79">
       <c r="B79" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>111</v>
+        <v>193</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E79" s="1"/>
+        <v>183</v>
+      </c>
       <c r="F79" s="1">
-        <v>18.4</v>
+        <v>6.5</v>
+      </c>
+      <c r="J79" s="2" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="80">
       <c r="B80" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F80" s="1">
-        <v>17.0</v>
+        <v>195</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="J80" s="2" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="81">
       <c r="B81" s="1" t="s">
-        <v>114</v>
+        <v>197</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>51</v>
+        <v>34</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="82">
       <c r="B82" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F82" s="1">
-        <v>7.5</v>
+        <v>202</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="83">
       <c r="B83" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F83" s="1">
-        <v>6.5</v>
+        <v>206</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="84">
       <c r="B84" s="1" t="s">
-        <v>117</v>
+        <v>206</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J86" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="B87" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J87" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F88" s="3">
+        <v>45514.0</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="B89" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F89" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J89" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="B90" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F90" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I90" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J90" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="B91" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F91" s="1">
+        <v>17.0</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="J91" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F92" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J92" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F93" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F94" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I94" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="B95" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F95" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F96" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="B97" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="B98" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F98" s="3">
+        <v>45481.0</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="B99" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="B100" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="K100" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H103" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="J103" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H104" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I104" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="J104" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="B105" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="J105" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="B106" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G106" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="I106" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="J106" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="B107" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E107" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="B108" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="B109" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="B110" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="B111" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="B112" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I112" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J112" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="B113" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F113" s="1">
+        <v>28.99</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="B114" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F114" s="1">
+        <v>28.99</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="J114" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="B115" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F115" s="1">
+        <v>28.99</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="I115" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="J115" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="B116" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F116" s="1">
+        <v>28.99</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="I116" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="J116" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="B117" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F117" s="1">
+        <v>28.99</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="I117" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="J117" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="B118" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F118" s="1">
+        <v>28.99</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="I118" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="B119" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F119" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I119" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J119" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="B120" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F120" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I120" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J120" s="4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="B121" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F121" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="I121" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J121" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="B122" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F122" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I122" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J122" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="B123" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F123" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I123" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J123" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="B124" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I124" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J124" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="B125" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J125" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="B126" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F126" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H126" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I126" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J126" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="B127" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F127" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I127" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J127" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="B128" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F128" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="H128" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="I128" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J128" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="B129" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F129" s="3">
+        <v>45577.0</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="J129" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="B130" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="F130" s="1">
+        <v>15.5</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="H130" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="I130" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J130" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="B131" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F131" s="1">
+        <v>15.5</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="H131" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="I131" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J131" s="1" t="s">
+        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>